<commit_message>
upates to bc08_cas and nb01_lyr markdown files.
</commit_message>
<xml_diff>
--- a/data/cas_attributes.xlsx
+++ b/data/cas_attributes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20342"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20348"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2ADA20-C0C5-4905-84E5-F124042C666B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89ADD941-F832-4FFA-9875-302D987D84CC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5090" yWindow="480" windowWidth="20840" windowHeight="15560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5090" yWindow="480" windowWidth="20840" windowHeight="15560" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="7" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2812" uniqueCount="925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="925">
   <si>
     <t>CATEGORY</t>
   </si>
@@ -9346,7 +9346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -10386,7 +10386,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="9" t="s">
         <v>922</v>
       </c>
     </row>
@@ -10556,6 +10556,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10563,7 +10564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD919EF5-0DF1-48F5-873B-2A0A1D4FEBB0}">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>